<commit_message>
added sensitivity of bimodality test to data sets (Appendix D)
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="12405" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="12405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>Model</t>
   </si>
@@ -167,6 +167,64 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>Maximum value of floating plant cover used</t>
+  </si>
+  <si>
+    <t>Minimum value of floating plant cover used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterbodies that change aquatic plant state removed </t>
+  </si>
+  <si>
+    <t>Segment 1: &lt;0.0.3004 mg P/L</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segment 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0.03698 mg P/L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segment 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0.03004 mg P/L</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -176,7 +234,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -240,6 +298,32 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -483,7 +567,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -532,12 +616,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="214">
@@ -1056,7 +1161,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A2" sqref="A2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1221,15 +1326,438 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="22" style="23" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="26">
+        <v>51</v>
+      </c>
+      <c r="D3" s="26">
+        <v>43.713000000000001</v>
+      </c>
+      <c r="E3" s="26">
+        <v>69.397999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="26">
+        <v>49</v>
+      </c>
+      <c r="D4" s="26">
+        <v>42.384</v>
+      </c>
+      <c r="E4" s="26">
+        <v>69.090999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26">
+        <v>12</v>
+      </c>
+      <c r="D5" s="26">
+        <v>8.7729999999999997</v>
+      </c>
+      <c r="E5" s="26">
+        <v>20.846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26">
+        <v>37</v>
+      </c>
+      <c r="D6" s="26">
+        <v>31.318000000000001</v>
+      </c>
+      <c r="E6" s="26">
+        <v>46.261000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="26">
+        <v>49</v>
+      </c>
+      <c r="D7" s="28">
+        <f>SUM(D8:D9)</f>
+        <v>11.783200000000001</v>
+      </c>
+      <c r="E7" s="28">
+        <f>SUM(E8:E9)</f>
+        <v>27.089599999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26">
+        <v>18</v>
+      </c>
+      <c r="D8" s="28">
+        <v>3.22</v>
+      </c>
+      <c r="E8" s="26">
+        <v>6.4105999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26">
+        <v>31</v>
+      </c>
+      <c r="D9" s="26">
+        <v>8.5632000000000001</v>
+      </c>
+      <c r="E9" s="26">
+        <v>20.678999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="26">
+        <v>51</v>
+      </c>
+      <c r="D13" s="26">
+        <v>41.271999999999998</v>
+      </c>
+      <c r="E13" s="26">
+        <v>63.734999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="26">
+        <v>51</v>
+      </c>
+      <c r="D14" s="26">
+        <v>38.4</v>
+      </c>
+      <c r="E14" s="26">
+        <v>63.734999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26">
+        <v>10</v>
+      </c>
+      <c r="D15" s="26">
+        <v>7.9535999999999998</v>
+      </c>
+      <c r="E15" s="26">
+        <v>17.510999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26">
+        <v>39</v>
+      </c>
+      <c r="D16" s="26">
+        <v>33.015000000000001</v>
+      </c>
+      <c r="E16" s="26">
+        <v>50.009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="26">
+        <v>49</v>
+      </c>
+      <c r="D17" s="28">
+        <f>SUM(D18:D19)</f>
+        <v>12.2264</v>
+      </c>
+      <c r="E17" s="28">
+        <f>SUM(E18:E19)</f>
+        <v>31.603899999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26">
+        <v>10</v>
+      </c>
+      <c r="D18" s="28">
+        <v>1.8794</v>
+      </c>
+      <c r="E18" s="26">
+        <v>4.9999000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26">
+        <v>39</v>
+      </c>
+      <c r="D19" s="26">
+        <v>10.347</v>
+      </c>
+      <c r="E19" s="26">
+        <v>26.603999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="26">
+        <v>43</v>
+      </c>
+      <c r="D23" s="26">
+        <v>33.695</v>
+      </c>
+      <c r="E23" s="26">
+        <v>53.686999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="26">
+        <v>43</v>
+      </c>
+      <c r="D24" s="26">
+        <v>33.695</v>
+      </c>
+      <c r="E24" s="26">
+        <v>53.686999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="26">
+        <v>8</v>
+      </c>
+      <c r="D25" s="26">
+        <v>6.4013</v>
+      </c>
+      <c r="E25" s="26">
+        <v>13.162000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="26">
+        <v>33</v>
+      </c>
+      <c r="D26" s="26">
+        <v>23.824999999999999</v>
+      </c>
+      <c r="E26" s="26">
+        <v>37.628</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="26">
+        <v>49</v>
+      </c>
+      <c r="D27" s="28">
+        <f>SUM(D28:D29)</f>
+        <v>10.275500000000001</v>
+      </c>
+      <c r="E27" s="28">
+        <f>SUM(E28:E29)</f>
+        <v>25.678899999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="26">
+        <v>10</v>
+      </c>
+      <c r="D28" s="28">
+        <v>1.8794</v>
+      </c>
+      <c r="E28" s="26">
+        <v>4.9999000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="26">
+        <v>31</v>
+      </c>
+      <c r="D29" s="26">
+        <v>8.3961000000000006</v>
+      </c>
+      <c r="E29" s="26">
+        <v>20.678999999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1237,7 +1765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -1268,23 +1796,23 @@
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
     </row>
     <row r="2" spans="1:16" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -1687,7 +2215,7 @@
       <c r="D1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="F1" s="14" t="s">
@@ -1707,7 +2235,7 @@
       <c r="D2" s="11">
         <v>0.4</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="18">
         <v>40974</v>
       </c>
       <c r="F2" s="8">
@@ -1727,7 +2255,7 @@
       <c r="D3" s="11">
         <v>0.59</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="18">
         <v>40967</v>
       </c>
       <c r="F3" s="8">
@@ -1747,7 +2275,7 @@
       <c r="D4" s="11">
         <v>1.61</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="18">
         <v>40966</v>
       </c>
       <c r="F4" s="8">
@@ -1767,7 +2295,7 @@
       <c r="D5" s="11">
         <v>1.5</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>40966</v>
       </c>
       <c r="F5" s="8">
@@ -1787,7 +2315,7 @@
       <c r="D6" s="11">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <v>40966</v>
       </c>
       <c r="F6" s="8">
@@ -1807,7 +2335,7 @@
       <c r="D7" s="11">
         <v>0.36</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>40966</v>
       </c>
       <c r="F7" s="8">
@@ -1827,7 +2355,7 @@
       <c r="D8" s="11">
         <v>0.1</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>40967</v>
       </c>
       <c r="F8" s="8">
@@ -1847,7 +2375,7 @@
       <c r="D9" s="11">
         <v>3.34</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <v>40980</v>
       </c>
       <c r="F9" s="8">
@@ -1867,7 +2395,7 @@
       <c r="D10" s="11">
         <v>4.3899999999999997</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <v>40980</v>
       </c>
       <c r="F10" s="10">

</xml_diff>

<commit_message>
re-vised table for manuscript
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="12405" activeTab="1"/>
+    <workbookView xWindow="18630" yWindow="150" windowWidth="10170" windowHeight="13245"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
   <si>
     <t>Model</t>
   </si>
@@ -59,35 +59,6 @@
   </si>
   <si>
     <t>Segment 1: &lt;0.0.3698 mg P/L</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Segment 2: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>≥</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>0.03698 mg P/L</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT ADDITIVE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSURE IF THESE SHOULD BE ADDED </t>
   </si>
   <si>
     <t>df</t>
@@ -225,16 +196,26 @@
       <t>0.03004 mg P/L</t>
     </r>
   </si>
+  <si>
+    <t>Latent class beta regression</t>
+  </si>
+  <si>
+    <t>breakpoint at 0.03004 mg P /L</t>
+  </si>
+  <si>
+    <t>2 clusters</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -253,12 +234,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -297,12 +272,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -353,221 +322,221 @@
   </borders>
   <cellStyleXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -588,61 +557,67 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="214">
@@ -1158,23 +1133,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="6"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="6.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1182,16 +1156,13 @@
         <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1199,16 +1170,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="6">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="D2" s="6">
-        <v>43.713000000000001</v>
-      </c>
-      <c r="E2" s="6">
-        <v>69.397999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>95.40164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1216,107 +1184,55 @@
         <v>8</v>
       </c>
       <c r="C3" s="6">
-        <v>49</v>
-      </c>
-      <c r="D3" s="6">
-        <v>42.384</v>
-      </c>
-      <c r="E3" s="6">
-        <v>69.090999999999994</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31">
+        <v>101.4798</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6">
-        <v>8.7729999999999997</v>
-      </c>
-      <c r="E4" s="6">
-        <v>20.846</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="31"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D5" s="6">
-        <v>31.318000000000001</v>
-      </c>
-      <c r="E5" s="6">
-        <v>46.261000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7">
-        <f>SUM(D7:D8)</f>
-        <v>11.783200000000001</v>
-      </c>
-      <c r="E6" s="7">
-        <f>SUM(E7:E8)</f>
-        <v>27.089599999999997</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6">
-        <v>18</v>
-      </c>
-      <c r="D7" s="7">
-        <v>3.22</v>
-      </c>
-      <c r="E7" s="6">
-        <v>6.4105999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6">
-        <v>31</v>
-      </c>
-      <c r="D8" s="6">
-        <v>8.5632000000000001</v>
-      </c>
-      <c r="E8" s="6">
-        <v>20.678999999999998</v>
-      </c>
+        <v>-328.6841</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1328,430 +1244,430 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="22" style="23" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="25.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="22" style="22" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>43</v>
+      <c r="A1" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>51</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>43.713000000000001</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>69.397999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>49</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="25">
         <v>42.384</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="25">
         <v>69.090999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25">
         <v>12</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>8.7729999999999997</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>20.846</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26">
+      <c r="A6" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25">
         <v>37</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25">
         <v>31.318000000000001</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="25">
         <v>46.261000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>49</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <f>SUM(D8:D9)</f>
         <v>11.783200000000001</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <f>SUM(E8:E9)</f>
         <v>27.089599999999997</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25">
         <v>18</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <v>3.22</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="25">
         <v>6.4105999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26">
+      <c r="B9" s="25"/>
+      <c r="C9" s="25">
         <v>31</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="25">
         <v>8.5632000000000001</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="25">
         <v>20.678999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>44</v>
+      <c r="A11" s="21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="25">
         <v>51</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="25">
         <v>41.271999999999998</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="25">
         <v>63.734999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="25">
         <v>51</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="25">
         <v>38.4</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="25">
         <v>63.734999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26">
+      <c r="A15" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25">
         <v>10</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="25">
         <v>7.9535999999999998</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="25">
         <v>17.510999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26">
+      <c r="A16" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25">
         <v>39</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="25">
         <v>33.015000000000001</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="25">
         <v>50.009</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="25">
         <v>49</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <f>SUM(D18:D19)</f>
         <v>12.2264</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="27">
         <f>SUM(E18:E19)</f>
         <v>31.603899999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26">
+      <c r="B18" s="25"/>
+      <c r="C18" s="25">
         <v>10</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="27">
         <v>1.8794</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="25">
         <v>4.9999000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26">
+      <c r="B19" s="25"/>
+      <c r="C19" s="25">
         <v>39</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="25">
         <v>10.347</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="25">
         <v>26.603999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="25">
+        <v>43</v>
+      </c>
+      <c r="D23" s="25">
+        <v>33.695</v>
+      </c>
+      <c r="E23" s="25">
+        <v>53.686999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="25">
+        <v>43</v>
+      </c>
+      <c r="D24" s="25">
+        <v>33.695</v>
+      </c>
+      <c r="E24" s="25">
+        <v>53.686999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="25">
+        <v>8</v>
+      </c>
+      <c r="D25" s="25">
+        <v>6.4013</v>
+      </c>
+      <c r="E25" s="25">
+        <v>13.162000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="26">
-        <v>43</v>
-      </c>
-      <c r="D23" s="26">
-        <v>33.695</v>
-      </c>
-      <c r="E23" s="26">
-        <v>53.686999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="26">
-        <v>43</v>
-      </c>
-      <c r="D24" s="26">
-        <v>33.695</v>
-      </c>
-      <c r="E24" s="26">
-        <v>53.686999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="26">
-        <v>8</v>
-      </c>
-      <c r="D25" s="26">
-        <v>6.4013</v>
-      </c>
-      <c r="E25" s="26">
-        <v>13.162000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="26">
+      <c r="C26" s="25">
         <v>33</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="25">
         <v>23.824999999999999</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="25">
         <v>37.628</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="25">
         <v>49</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="27">
         <f>SUM(D28:D29)</f>
         <v>10.275500000000001</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="27">
         <f>SUM(E28:E29)</f>
         <v>25.678899999999999</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="25">
         <v>10</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="27">
         <v>1.8794</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="25">
         <v>4.9999000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="25">
         <v>31</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="25">
         <v>8.3961000000000006</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="25">
         <v>20.678999999999998</v>
       </c>
     </row>
@@ -1796,71 +1712,71 @@
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="F1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="J1" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="N1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M2" s="15"/>
       <c r="N2" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="10">
         <v>40.884217</v>
@@ -1900,7 +1816,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" s="10">
         <v>41.090580000000003</v>
@@ -1938,7 +1854,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" s="10">
         <v>40.944353</v>
@@ -1978,7 +1894,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="10">
         <v>41.824159999999999</v>
@@ -2016,7 +1932,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="10">
         <v>40.764775</v>
@@ -2056,7 +1972,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="10">
         <v>40.967677000000002</v>
@@ -2092,7 +2008,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="10">
         <v>41.078069999999997</v>
@@ -2130,7 +2046,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="10">
         <v>41.270328999999997</v>
@@ -2188,7 +2104,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,27 +2120,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="10">
         <v>40.962400000000002</v>
@@ -2244,7 +2160,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="10">
         <v>40.884217</v>
@@ -2264,7 +2180,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="10">
         <v>40.844799999999999</v>
@@ -2284,7 +2200,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="10">
         <v>40.9465</v>
@@ -2304,7 +2220,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="10">
         <v>40.944353</v>
@@ -2324,7 +2240,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10">
         <v>40.897199999999998</v>
@@ -2344,7 +2260,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" s="10">
         <v>40.857399999999998</v>
@@ -2364,7 +2280,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="10">
         <v>40.764775</v>
@@ -2384,7 +2300,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="10">
         <v>40.7699</v>

</xml_diff>

<commit_message>
dataFP in main text; dataFPsmall in appendix
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>Model</t>
   </si>
@@ -205,6 +205,9 @@
   <si>
     <t>2 clusters</t>
   </si>
+  <si>
+    <t>breakpoint at 0.03698 mg P /L</t>
+  </si>
 </sst>
 </file>
 
@@ -215,7 +218,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -293,6 +296,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -536,7 +545,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,13 +619,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1133,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A1:D6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1172,8 +1187,8 @@
       <c r="C2" s="6">
         <v>2</v>
       </c>
-      <c r="D2" s="6">
-        <v>95.40164</v>
+      <c r="D2" s="32">
+        <v>95.405799999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,8 +1201,8 @@
       <c r="C3" s="6">
         <v>5</v>
       </c>
-      <c r="D3" s="31">
-        <v>101.4798</v>
+      <c r="D3" s="32">
+        <v>93.182100000000005</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,10 +1211,10 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="31"/>
+      <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1229,10 +1244,76 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="33">
+        <v>70.246589999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5</v>
+      </c>
+      <c r="D11" s="33">
+        <v>69.681229999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-86.378600000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1712,23 +1793,23 @@
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
getting the appendices right!
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Appendix E1" sheetId="2" r:id="rId2"/>
-    <sheet name="Appendix E2" sheetId="3" r:id="rId3"/>
-    <sheet name="Appendix A1" sheetId="4" r:id="rId4"/>
+    <sheet name="Appendix A1" sheetId="4" r:id="rId2"/>
+    <sheet name="Appendix  D" sheetId="5" r:id="rId3"/>
+    <sheet name="Appendix E1" sheetId="3" r:id="rId4"/>
+    <sheet name="Appendix E2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="44">
   <si>
     <t>Model</t>
   </si>
@@ -142,10 +143,24 @@
     <t>breakpoint at 0.03698 mg P /L</t>
   </si>
   <si>
-    <t>dataFPsmall</t>
-  </si>
-  <si>
     <t>dataFP</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ponds with floating plants present </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(n = 96)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ponds &lt;5 ha. with floating plants present</t>
   </si>
 </sst>
 </file>
@@ -157,7 +172,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -234,6 +249,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -483,7 +504,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -548,14 +569,17 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="214">
@@ -1071,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1169,80 +1193,6 @@
       <c r="A8" s="3"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="6">
-        <v>2</v>
-      </c>
-      <c r="D10" s="23">
-        <v>70.246589999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="6">
-        <v>5</v>
-      </c>
-      <c r="D11" s="23">
-        <v>69.681229999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6">
-        <v>-86.378600000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1252,246 +1202,222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="A1:D24"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.28515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="31.28515625" style="27"/>
-    <col min="3" max="3" width="2.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="31.28515625" style="27"/>
+    <col min="1" max="1" width="18.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="17"/>
+    <col min="3" max="3" width="10.28515625" style="17" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="17"/>
+    <col min="6" max="6" width="14.42578125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="17" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="D3" s="22">
-        <v>95.405799999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6">
-        <v>5</v>
-      </c>
-      <c r="D4" s="22">
-        <v>93.182100000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6">
-        <v>-328.6841</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6">
-        <v>2</v>
-      </c>
-      <c r="D11" s="21">
-        <v>80.461929999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="6">
-        <v>5</v>
-      </c>
-      <c r="D12" s="28"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="6">
-        <v>7</v>
-      </c>
-      <c r="D14" s="21">
-        <v>-334.96749999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6">
-        <v>2</v>
-      </c>
-      <c r="D20" s="21">
-        <v>70.894829999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="6">
-        <v>5</v>
-      </c>
-      <c r="D21" s="28"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="6">
-        <v>7</v>
-      </c>
-      <c r="D23" s="21">
-        <v>-327.06639999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+    <row r="1" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="10">
+        <v>40.962400000000002</v>
+      </c>
+      <c r="C2" s="10">
+        <v>-73.128500000000003</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="E2" s="18">
+        <v>40974</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.38663999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="10">
+        <v>40.884217</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-73.361185000000006</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="E3" s="18">
+        <v>40967</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1.9720000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="10">
+        <v>40.844799999999999</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-73.139200000000002</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1.61</v>
+      </c>
+      <c r="E4" s="18">
+        <v>40966</v>
+      </c>
+      <c r="F4" s="8">
+        <v>3.6979999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="10">
+        <v>40.9465</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-73.115600000000001</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="18">
+        <v>40966</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2.579E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="10">
+        <v>40.944353</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-73.116020000000006</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E6" s="18">
+        <v>40966</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2.366E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="10">
+        <v>40.897199999999998</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-73.148300000000006</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.36</v>
+      </c>
+      <c r="E7" s="18">
+        <v>40966</v>
+      </c>
+      <c r="F7" s="8">
+        <v>8.8620000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="10">
+        <v>40.857399999999998</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-73.210300000000004</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="18">
+        <v>40967</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1.7680000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="10">
+        <v>40.764775</v>
+      </c>
+      <c r="C9" s="10">
+        <v>-72.982065000000006</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3.34</v>
+      </c>
+      <c r="E9" s="18">
+        <v>40980</v>
+      </c>
+      <c r="F9" s="8">
+        <v>3.5229999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="10">
+        <v>40.7699</v>
+      </c>
+      <c r="C10" s="10">
+        <v>-72.993200000000002</v>
+      </c>
+      <c r="D10" s="11">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="E10" s="18">
+        <v>40980</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2.2200000000000001E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1501,10 +1427,195 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31" style="28" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="11" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="22">
+        <v>95.405799999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+      <c r="D4" s="22">
+        <v>93.182100000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>-328.6841</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="23">
+        <v>70.246589999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="23">
+        <v>69.681229999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6">
+        <v>-86.378600000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1534,23 +1645,23 @@
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
     </row>
     <row r="2" spans="1:16" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -1921,224 +2032,248 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="31.28515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="17"/>
-    <col min="3" max="3" width="10.28515625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="17"/>
-    <col min="6" max="6" width="14.42578125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="17" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="2" width="31.28515625" style="25"/>
+    <col min="3" max="3" width="2.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="31.28515625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="10">
-        <v>40.962400000000002</v>
-      </c>
-      <c r="C2" s="10">
-        <v>-73.128500000000003</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="E2" s="18">
-        <v>40974</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0.38663999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="10">
-        <v>40.884217</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-73.361185000000006</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0.59</v>
-      </c>
-      <c r="E3" s="18">
-        <v>40967</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1.9720000000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="10">
-        <v>40.844799999999999</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-73.139200000000002</v>
-      </c>
-      <c r="D4" s="11">
-        <v>1.61</v>
-      </c>
-      <c r="E4" s="18">
-        <v>40966</v>
-      </c>
-      <c r="F4" s="8">
-        <v>3.6979999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="10">
-        <v>40.9465</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-73.115600000000001</v>
-      </c>
-      <c r="D5" s="11">
-        <v>1.5</v>
-      </c>
-      <c r="E5" s="18">
-        <v>40966</v>
-      </c>
-      <c r="F5" s="8">
-        <v>2.579E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="10">
-        <v>40.944353</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-73.116020000000006</v>
-      </c>
-      <c r="D6" s="11">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="E6" s="18">
-        <v>40966</v>
-      </c>
-      <c r="F6" s="8">
-        <v>2.366E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="10">
-        <v>40.897199999999998</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-73.148300000000006</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0.36</v>
-      </c>
-      <c r="E7" s="18">
-        <v>40966</v>
-      </c>
-      <c r="F7" s="8">
-        <v>8.8620000000000004E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="10">
-        <v>40.857399999999998</v>
-      </c>
-      <c r="C8" s="10">
-        <v>-73.210300000000004</v>
-      </c>
-      <c r="D8" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="18">
-        <v>40967</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1.7680000000000001E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="10">
-        <v>40.764775</v>
-      </c>
-      <c r="C9" s="10">
-        <v>-72.982065000000006</v>
-      </c>
-      <c r="D9" s="11">
-        <v>3.34</v>
-      </c>
-      <c r="E9" s="18">
-        <v>40980</v>
-      </c>
-      <c r="F9" s="8">
-        <v>3.5229999999999997E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="10">
-        <v>40.7699</v>
-      </c>
-      <c r="C10" s="10">
-        <v>-72.993200000000002</v>
-      </c>
-      <c r="D10" s="11">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="E10" s="18">
-        <v>40980</v>
-      </c>
-      <c r="F10" s="10">
-        <v>2.2200000000000001E-2</v>
-      </c>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="22">
+        <v>95.405799999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+      <c r="D4" s="22">
+        <v>93.182100000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>-328.6841</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="21">
+        <v>80.461929999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="26"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6">
+        <v>7</v>
+      </c>
+      <c r="D14" s="21">
+        <v>-334.96749999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2</v>
+      </c>
+      <c r="D20" s="21">
+        <v>70.894829999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="6">
+        <v>5</v>
+      </c>
+      <c r="D21" s="26"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="6">
+        <v>7</v>
+      </c>
+      <c r="D23" s="21">
+        <v>-327.06639999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>